<commit_message>
Updated the tables in the results section even more and cleaned them up a little bit.
</commit_message>
<xml_diff>
--- a/data/layton_08_17_2020.xlsx
+++ b/data/layton_08_17_2020.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="68" documentId="8_{253146AB-F60D-454D-BFC2-97651184C691}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5458837B-9CE9-4B95-8E90-58B5A951E08F}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F4527FA2-9E94-429F-8CD3-417190D35048}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F4527FA2-9E94-429F-8CD3-417190D35048}"/>
   </bookViews>
   <sheets>
     <sheet name="08-17-2020" sheetId="1" r:id="rId1"/>
@@ -514,8 +514,8 @@
   <dimension ref="A1:AM2130"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X5" sqref="X5"/>
+      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X4" sqref="X4:X154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>